<commit_message>
CentralizatorVechimeComplet contains Hiring Date
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/Centralizator pe vechime complet.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/Centralizator pe vechime complet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandru POP\Desktop\Proiecte\webapp-spring\server\src\main\java\net\guides\springboot2\crud\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\webapp-spring\server\src\main\java\net\guides\springboot2\crud\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FA3AD0-5E3A-47C7-93D8-2B55AD88DBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="7800" tabRatio="334"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="334" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Numar</t>
   </si>
@@ -70,12 +71,15 @@
   </si>
   <si>
     <t>Vechime</t>
+  </si>
+  <si>
+    <t>Data angajării</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -159,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -182,6 +186,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -497,11 +507,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -515,35 +525,36 @@
     <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.88671875"/>
-    <col min="11" max="12" width="9.5546875"/>
+    <col min="11" max="11" width="12.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
@@ -552,7 +563,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
       <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
@@ -560,11 +571,11 @@
       <c r="F7" s="8"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -595,12 +606,15 @@
       <c r="J10" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="K10" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D6:F6"/>

</xml_diff>